<commit_message>
get the data from redis
</commit_message>
<xml_diff>
--- a/doc/redis-test.xlsx
+++ b/doc/redis-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OpenSource\redis-rtd\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navni\source\repos\nsharmanahellc\nme-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B399D66D-3ED8-4DB7-BA9A-BB957F6F4A46}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0A78F6-22EE-409A-A3F8-836EF039CE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="7005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,20 @@
     <definedName name="FIELD">Sheet1!#REF!</definedName>
     <definedName name="progId">Sheet1!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -154,6 +164,7 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -180,146 +191,132 @@
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
     <main first="redis">
-      <tp>
-        <v>7891</v>
-        <stp/>
-        <stp>localhost</stp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
+        <stp>RAW_2</stp>
+        <stp/>
+        <tr r="C12" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
+        <stp>RAW_0</stp>
+        <stp/>
+        <tr r="C10" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
+        <stp>RAW_1</stp>
+        <stp/>
+        <tr r="C11" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
         <stp>JSON_2</stp>
-        <stp>len</stp>
-        <tr r="E7" s="1"/>
-      </tp>
-      <tp>
-        <v>0</v>
-        <stp/>
-        <stp>localhost</stp>
+        <stp>padding</stp>
+        <tr r="F7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
         <stp>JSON_0</stp>
-        <stp>len</stp>
-        <tr r="E5" s="1"/>
-      </tp>
-      <tp>
-        <v>6346</v>
-        <stp/>
-        <stp>localhost</stp>
+        <stp>padding</stp>
+        <tr r="F5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
         <stp>JSON_1</stp>
-        <stp>len</stp>
-        <tr r="E6" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>JSON_1</v>
-        <stp/>
-        <stp>localhost</stp>
+        <stp>padding</stp>
+        <tr r="F6" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
+        <stp>JSON_0</stp>
+        <tr r="G5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
+        <stp>JSON_0</stp>
+        <stp>channel</stp>
+        <tr r="C5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
         <stp>JSON_1</stp>
         <stp>channel</stp>
         <tr r="C6" s="1"/>
       </tp>
       <tp t="s">
-        <v>JSON_0</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>JSON_0</stp>
-        <stp>channel</stp>
-        <tr r="C5" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>JSON_2</v>
-        <stp/>
-        <stp>localhost</stp>
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
         <stp>JSON_2</stp>
         <stp>channel</stp>
         <tr r="C7" s="1"/>
       </tp>
       <tp t="s">
-        <v>{ "channel": "JSON_0", "FIELD": 30716, "len": 0, "padding": ""}</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>JSON_0</stp>
-        <tr r="G5" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>{ "channel": "JSON_1", "FIELD": 30717, "len": 6346, "padding": "xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx"}</v>
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>JSON_1</stp>
         <tr r="G6" s="1"/>
       </tp>
       <tp t="s">
-        <v>{ "channel": "JSON_2", "FIELD": 30718, "len": 7891, "padding": "xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx"}</v>
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>localhost</stp>
         <stp>JSON_2</stp>
         <tr r="G7" s="1"/>
       </tp>
       <tp t="s">
-        <v>xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>JSON_2</stp>
-        <stp>padding</stp>
-        <tr r="F7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>JSON_1</stp>
-        <stp>padding</stp>
-        <tr r="F6" s="1"/>
-      </tp>
-      <tp t="s">
-        <v/>
-        <stp/>
-        <stp>localhost</stp>
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
+        <stp>&lt;?&gt;</stp>
+        <stp>len</stp>
+        <tr r="E7" s="1"/>
+        <tr r="E6" s="1"/>
+        <tr r="E5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
         <stp>JSON_0</stp>
-        <stp>padding</stp>
-        <tr r="F5" s="1"/>
-      </tp>
-      <tp>
-        <v>30717</v>
-        <stp/>
-        <stp>localhost</stp>
+        <stp>FIELD</stp>
+        <tr r="D5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
         <stp>JSON_1</stp>
         <stp>FIELD</stp>
         <tr r="D6" s="1"/>
       </tp>
-      <tp>
-        <v>30716</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>JSON_0</stp>
-        <stp>FIELD</stp>
-        <tr r="D5" s="1"/>
-      </tp>
-      <tp>
-        <v>30718</v>
-        <stp/>
-        <stp>localhost</stp>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
+        <stp/>
+        <stp>192.168.0.59</stp>
         <stp>JSON_2</stp>
         <stp>FIELD</stp>
         <tr r="D7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>{ "channel": "RAW_2", "FIELD": 30717, "len": 2922, "padding": "xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx"}</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>RAW_2</stp>
-        <stp/>
-        <tr r="C12" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>{ "channel": "RAW_1", "FIELD": 30716, "len": 250, "padding": "xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx"}</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>RAW_1</stp>
-        <stp/>
-        <tr r="C11" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>{ "channel": "RAW_0", "FIELD": 30716, "len": 0, "padding": ""}</v>
-        <stp/>
-        <stp>localhost</stp>
-        <stp>RAW_0</stp>
-        <stp/>
-        <tr r="C10" s="1"/>
       </tp>
     </main>
   </volType>
@@ -332,16 +329,16 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Chan"/>
     <tableColumn id="4" xr3:uid="{26BD59B5-3D9A-4D57-8D5C-103D60ED8788}" name="channel" dataDxfId="3">
-      <calculatedColumnFormula>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[channel]])</calculatedColumnFormula>
+      <calculatedColumnFormula>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[channel]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="FIELD" dataDxfId="2">
-      <calculatedColumnFormula>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[FIELD]])</calculatedColumnFormula>
+      <calculatedColumnFormula>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[FIELD]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{9FA3B82A-3F7C-4441-88E7-0C903B64ABAB}" name="len" dataDxfId="1">
-      <calculatedColumnFormula>RTD(progId,,"localhost",Table1[[#This Row],[channel]],Table1[[#Headers],[len]])</calculatedColumnFormula>
+      <calculatedColumnFormula>RTD(progId,,"192.168.0.59",Table1[[#This Row],[channel]],Table1[[#Headers],[len]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{BD13D85A-4C00-4B1F-95DE-A970E6992D92}" name="padding" dataDxfId="0">
-      <calculatedColumnFormula>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[padding]])</calculatedColumnFormula>
+      <calculatedColumnFormula>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[padding]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -649,12 +646,12 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
@@ -697,24 +694,24 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[channel]])</f>
-        <v>JSON_0</v>
-      </c>
-      <c r="D5" s="2">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[FIELD]])</f>
-        <v>30716</v>
-      </c>
-      <c r="E5" s="2">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[channel]],Table1[[#Headers],[len]])</f>
-        <v>0</v>
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[channel]])</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[FIELD]])</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[channel]],Table1[[#Headers],[len]])</f>
+        <v>&lt;?&gt;</v>
       </c>
       <c r="F5" s="2" t="str">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[padding]])</f>
-        <v/>
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[padding]])</f>
+        <v>&lt;?&gt;</v>
       </c>
       <c r="G5" t="str">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]])</f>
-        <v>{ "channel": "JSON_0", "FIELD": 30716, "len": 0, "padding": ""}</v>
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]])</f>
+        <v>&lt;?&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -722,24 +719,24 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="str">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[channel]])</f>
-        <v>JSON_1</v>
-      </c>
-      <c r="D6" s="2">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[FIELD]])</f>
-        <v>30717</v>
-      </c>
-      <c r="E6" s="2">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[channel]],Table1[[#Headers],[len]])</f>
-        <v>6346</v>
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[channel]])</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[FIELD]])</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[channel]],Table1[[#Headers],[len]])</f>
+        <v>&lt;?&gt;</v>
       </c>
       <c r="F6" s="2" t="str">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[padding]])</f>
-        <v>xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx</v>
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[padding]])</f>
+        <v>&lt;?&gt;</v>
       </c>
       <c r="G6" t="str">
         <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]])</f>
-        <v>{ "channel": "JSON_1", "FIELD": 30717, "len": 6346, "padding": "xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx"}</v>
+        <v>&lt;?&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -747,24 +744,24 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="str">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[channel]])</f>
-        <v>JSON_2</v>
-      </c>
-      <c r="D7" s="2">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[FIELD]])</f>
-        <v>30718</v>
-      </c>
-      <c r="E7" s="2">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[channel]],Table1[[#Headers],[len]])</f>
-        <v>7891</v>
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[channel]])</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[FIELD]])</f>
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[channel]],Table1[[#Headers],[len]])</f>
+        <v>&lt;?&gt;</v>
       </c>
       <c r="F7" s="2" t="str">
-        <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]],Table1[[#Headers],[padding]])</f>
-        <v>xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx</v>
+        <f>RTD(progId,,"192.168.0.59",Table1[[#This Row],[Chan]],Table1[[#Headers],[padding]])</f>
+        <v>&lt;?&gt;</v>
       </c>
       <c r="G7" t="str">
         <f>RTD(progId,,"localhost",Table1[[#This Row],[Chan]])</f>
-        <v>{ "channel": "JSON_2", "FIELD": 30718, "len": 7891, "padding": "xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx"}</v>
+        <v>&lt;?&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -780,8 +777,8 @@
         <v>8</v>
       </c>
       <c r="C10" t="str">
-        <f>RTD(progId,,"localhost",B10,"")</f>
-        <v>{ "channel": "RAW_0", "FIELD": 30716, "len": 0, "padding": ""}</v>
+        <f>RTD(progId,,"192.168.0.59",B10,"")</f>
+        <v>&lt;?&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -789,8 +786,8 @@
         <v>7</v>
       </c>
       <c r="C11" t="str">
-        <f>RTD(progId,,"localhost",B11,"")</f>
-        <v>{ "channel": "RAW_1", "FIELD": 30716, "len": 250, "padding": "xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx"}</v>
+        <f>RTD(progId,,"192.168.0.59",B11,"")</f>
+        <v>&lt;?&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -798,8 +795,8 @@
         <v>9</v>
       </c>
       <c r="C12" t="str">
-        <f>RTD(progId,,"localhost",B12,"")</f>
-        <v>{ "channel": "RAW_2", "FIELD": 30717, "len": 2922, "padding": "xxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxxx"}</v>
+        <f>RTD(progId,,"192.168.0.59",B12,"")</f>
+        <v>&lt;?&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>